<commit_message>
looking at diff in veg weights
</commit_message>
<xml_diff>
--- a/data/understory_veg_weight_raw.xlsx
+++ b/data/understory_veg_weight_raw.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinehayes/Google Drive/Projects/Reburns/Chapters/Flammabllity/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C285370B-463C-AC4E-AA54-85673082CD11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9D7DE3-1D84-DB44-B253-7A288AC1E069}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36700" yWindow="1300" windowWidth="28880" windowHeight="19440" xr2:uid="{FB673233-C73A-D447-B023-A040BAD96657}"/>
+    <workbookView xWindow="-80" yWindow="460" windowWidth="25640" windowHeight="14480" xr2:uid="{FB673233-C73A-D447-B023-A040BAD96657}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="108">
   <si>
     <t>SITE</t>
   </si>
@@ -307,6 +307,57 @@
   </si>
   <si>
     <t>STEESE</t>
+  </si>
+  <si>
+    <t>65_1</t>
+  </si>
+  <si>
+    <t>52_1</t>
+  </si>
+  <si>
+    <t>37_3</t>
+  </si>
+  <si>
+    <t>56_2</t>
+  </si>
+  <si>
+    <t>14_3</t>
+  </si>
+  <si>
+    <t>11_0</t>
+  </si>
+  <si>
+    <t>55_3</t>
+  </si>
+  <si>
+    <t>7_3</t>
+  </si>
+  <si>
+    <t>32_2</t>
+  </si>
+  <si>
+    <t>47_2</t>
+  </si>
+  <si>
+    <t>57_2</t>
+  </si>
+  <si>
+    <t>12_1</t>
+  </si>
+  <si>
+    <t>50_1</t>
+  </si>
+  <si>
+    <t>54_3</t>
+  </si>
+  <si>
+    <t>15_3</t>
+  </si>
+  <si>
+    <t>39_2</t>
+  </si>
+  <si>
+    <t>64_1</t>
   </si>
 </sst>
 </file>
@@ -660,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0FBA91F-253D-EE4D-B8FF-F1A098B04D6A}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91:F121"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,6 +744,12 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <v>191</v>
       </c>
@@ -708,6 +765,12 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3">
         <v>135</v>
       </c>
@@ -722,6 +785,12 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
       <c r="E4">
         <v>15</v>
       </c>
@@ -736,6 +805,12 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="E5">
         <v>115</v>
       </c>
@@ -750,6 +825,12 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
       <c r="E6">
         <v>45</v>
       </c>
@@ -764,6 +845,12 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
       <c r="E7">
         <v>82</v>
       </c>
@@ -778,6 +865,12 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8">
         <v>30</v>
       </c>
@@ -792,6 +885,12 @@
       <c r="B9" t="s">
         <v>13</v>
       </c>
+      <c r="C9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
       <c r="E9">
         <v>30</v>
       </c>
@@ -806,6 +905,12 @@
       <c r="B10" t="s">
         <v>14</v>
       </c>
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
       <c r="E10">
         <v>35</v>
       </c>
@@ -820,6 +925,12 @@
       <c r="B11" t="s">
         <v>15</v>
       </c>
+      <c r="C11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
       <c r="E11">
         <v>82</v>
       </c>
@@ -834,6 +945,12 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
       <c r="E12">
         <v>25</v>
       </c>
@@ -848,6 +965,12 @@
       <c r="B13" t="s">
         <v>17</v>
       </c>
+      <c r="C13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
       <c r="E13">
         <v>24</v>
       </c>
@@ -862,6 +985,12 @@
       <c r="B14" t="s">
         <v>18</v>
       </c>
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="E14">
         <v>77</v>
       </c>
@@ -876,6 +1005,12 @@
       <c r="B15" t="s">
         <v>19</v>
       </c>
+      <c r="C15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
       <c r="E15">
         <v>26</v>
       </c>
@@ -890,6 +1025,12 @@
       <c r="B16" t="s">
         <v>20</v>
       </c>
+      <c r="C16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
       <c r="E16">
         <v>51</v>
       </c>
@@ -904,6 +1045,12 @@
       <c r="B17" t="s">
         <v>21</v>
       </c>
+      <c r="C17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
       <c r="E17">
         <v>24</v>
       </c>
@@ -918,6 +1065,12 @@
       <c r="B18" t="s">
         <v>22</v>
       </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
       <c r="E18">
         <v>67</v>
       </c>
@@ -932,6 +1085,12 @@
       <c r="B19" t="s">
         <v>23</v>
       </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
       <c r="E19">
         <v>40</v>
       </c>
@@ -946,6 +1105,12 @@
       <c r="B20" t="s">
         <v>24</v>
       </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
       <c r="E20">
         <v>37</v>
       </c>
@@ -960,6 +1125,12 @@
       <c r="B21" t="s">
         <v>25</v>
       </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
       <c r="E21">
         <v>30</v>
       </c>
@@ -974,6 +1145,12 @@
       <c r="B22" t="s">
         <v>26</v>
       </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
       <c r="E22">
         <v>36</v>
       </c>
@@ -988,6 +1165,12 @@
       <c r="B23" t="s">
         <v>27</v>
       </c>
+      <c r="C23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
       <c r="E23">
         <v>37</v>
       </c>
@@ -1002,6 +1185,12 @@
       <c r="B24" t="s">
         <v>28</v>
       </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
       <c r="E24">
         <v>87</v>
       </c>
@@ -1016,6 +1205,12 @@
       <c r="B25" t="s">
         <v>29</v>
       </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
       <c r="E25">
         <v>36</v>
       </c>
@@ -1030,6 +1225,12 @@
       <c r="B26" t="s">
         <v>30</v>
       </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
       <c r="E26">
         <v>133</v>
       </c>
@@ -1044,6 +1245,12 @@
       <c r="B27" t="s">
         <v>31</v>
       </c>
+      <c r="C27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
       <c r="E27">
         <v>116</v>
       </c>
@@ -1058,6 +1265,12 @@
       <c r="B28" t="s">
         <v>32</v>
       </c>
+      <c r="C28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
       <c r="E28">
         <v>146</v>
       </c>
@@ -1072,6 +1285,12 @@
       <c r="B29" t="s">
         <v>33</v>
       </c>
+      <c r="C29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
       <c r="E29">
         <v>95</v>
       </c>
@@ -1086,6 +1305,12 @@
       <c r="B30" t="s">
         <v>34</v>
       </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
       <c r="E30">
         <v>30</v>
       </c>
@@ -1100,6 +1325,12 @@
       <c r="B31" t="s">
         <v>35</v>
       </c>
+      <c r="C31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
       <c r="E31">
         <v>80</v>
       </c>
@@ -1114,6 +1345,12 @@
       <c r="B32" t="s">
         <v>36</v>
       </c>
+      <c r="C32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
       <c r="E32">
         <v>77</v>
       </c>
@@ -1128,6 +1365,12 @@
       <c r="B33" t="s">
         <v>37</v>
       </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
       <c r="E33">
         <v>99</v>
       </c>
@@ -1142,6 +1385,12 @@
       <c r="B34" t="s">
         <v>38</v>
       </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
       <c r="E34">
         <v>43</v>
       </c>
@@ -1156,6 +1405,12 @@
       <c r="B35" t="s">
         <v>39</v>
       </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
       <c r="E35">
         <v>45</v>
       </c>
@@ -1170,6 +1425,12 @@
       <c r="B36" t="s">
         <v>40</v>
       </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
       <c r="E36">
         <v>76</v>
       </c>
@@ -1184,6 +1445,12 @@
       <c r="B37" t="s">
         <v>41</v>
       </c>
+      <c r="C37" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
       <c r="E37">
         <v>48</v>
       </c>
@@ -1195,6 +1462,12 @@
       <c r="B38" t="s">
         <v>42</v>
       </c>
+      <c r="C38" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
       <c r="E38">
         <v>47</v>
       </c>
@@ -1206,6 +1479,12 @@
       <c r="B39" t="s">
         <v>43</v>
       </c>
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
       <c r="E39">
         <v>56</v>
       </c>
@@ -1217,6 +1496,12 @@
       <c r="B40" t="s">
         <v>44</v>
       </c>
+      <c r="C40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
       <c r="E40">
         <v>22</v>
       </c>
@@ -1228,6 +1513,12 @@
       <c r="B41" t="s">
         <v>45</v>
       </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
       <c r="E41">
         <v>73</v>
       </c>
@@ -1238,6 +1529,12 @@
       </c>
       <c r="B42" t="s">
         <v>46</v>
+      </c>
+      <c r="C42" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
       </c>
       <c r="E42">
         <f>101+125</f>
@@ -1251,6 +1548,12 @@
       <c r="B43" t="s">
         <v>47</v>
       </c>
+      <c r="C43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
       <c r="E43">
         <v>75</v>
       </c>
@@ -1262,6 +1565,12 @@
       <c r="B44" t="s">
         <v>48</v>
       </c>
+      <c r="C44" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
       <c r="E44">
         <v>115</v>
       </c>
@@ -1273,6 +1582,12 @@
       <c r="B45" t="s">
         <v>15</v>
       </c>
+      <c r="C45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
       <c r="E45">
         <v>92</v>
       </c>
@@ -1284,6 +1599,12 @@
       <c r="B46" t="s">
         <v>49</v>
       </c>
+      <c r="C46" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
       <c r="E46">
         <v>165</v>
       </c>
@@ -1294,6 +1615,12 @@
       </c>
       <c r="B47" t="s">
         <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
       </c>
       <c r="E47">
         <f>66+97</f>
@@ -1307,6 +1634,12 @@
       <c r="B48" t="s">
         <v>51</v>
       </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
       <c r="E48">
         <v>101</v>
       </c>
@@ -1318,6 +1651,12 @@
       <c r="B49" t="s">
         <v>52</v>
       </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
       <c r="E49">
         <v>33</v>
       </c>
@@ -1329,6 +1668,12 @@
       <c r="B50" t="s">
         <v>29</v>
       </c>
+      <c r="C50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
       <c r="E50">
         <v>26</v>
       </c>
@@ -1340,6 +1685,12 @@
       <c r="B51" t="s">
         <v>53</v>
       </c>
+      <c r="C51" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
       <c r="E51">
         <v>50</v>
       </c>
@@ -1351,6 +1702,12 @@
       <c r="B52" t="s">
         <v>54</v>
       </c>
+      <c r="C52" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
       <c r="E52">
         <v>110</v>
       </c>
@@ -1362,6 +1719,12 @@
       <c r="B53" t="s">
         <v>55</v>
       </c>
+      <c r="C53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
       <c r="E53">
         <v>15</v>
       </c>
@@ -1373,6 +1736,12 @@
       <c r="B54" t="s">
         <v>56</v>
       </c>
+      <c r="C54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
       <c r="E54">
         <v>14</v>
       </c>
@@ -1384,6 +1753,12 @@
       <c r="B55" t="s">
         <v>57</v>
       </c>
+      <c r="C55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
       <c r="E55">
         <v>15</v>
       </c>
@@ -1395,6 +1770,12 @@
       <c r="B56" t="s">
         <v>58</v>
       </c>
+      <c r="C56" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
       <c r="E56">
         <v>40</v>
       </c>
@@ -1406,6 +1787,12 @@
       <c r="B57" t="s">
         <v>59</v>
       </c>
+      <c r="C57" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
       <c r="E57">
         <v>43</v>
       </c>
@@ -1417,6 +1804,12 @@
       <c r="B58" t="s">
         <v>60</v>
       </c>
+      <c r="C58" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
       <c r="E58">
         <v>12</v>
       </c>
@@ -1428,6 +1821,12 @@
       <c r="B59" t="s">
         <v>61</v>
       </c>
+      <c r="C59" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
       <c r="E59">
         <v>7</v>
       </c>
@@ -1439,6 +1838,12 @@
       <c r="B60" t="s">
         <v>62</v>
       </c>
+      <c r="C60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
       <c r="E60">
         <v>75</v>
       </c>
@@ -1450,6 +1855,12 @@
       <c r="B61" t="s">
         <v>63</v>
       </c>
+      <c r="C61" t="s">
+        <v>96</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
       <c r="E61">
         <v>28</v>
       </c>
@@ -1461,6 +1872,12 @@
       <c r="B62" t="s">
         <v>53</v>
       </c>
+      <c r="C62" t="s">
+        <v>106</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
       <c r="E62">
         <v>67</v>
       </c>
@@ -1472,6 +1889,12 @@
       <c r="B63" t="s">
         <v>64</v>
       </c>
+      <c r="C63" t="s">
+        <v>101</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
       <c r="E63">
         <v>22</v>
       </c>
@@ -1483,6 +1906,12 @@
       <c r="B64" t="s">
         <v>65</v>
       </c>
+      <c r="C64" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
       <c r="E64">
         <v>37</v>
       </c>
@@ -1494,6 +1923,12 @@
       <c r="B65" t="s">
         <v>66</v>
       </c>
+      <c r="C65" t="s">
+        <v>94</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
       <c r="E65">
         <v>29</v>
       </c>
@@ -1505,6 +1940,12 @@
       <c r="B66" t="s">
         <v>67</v>
       </c>
+      <c r="C66" t="s">
+        <v>101</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
       <c r="E66">
         <v>14</v>
       </c>
@@ -1516,6 +1957,12 @@
       <c r="B67" t="s">
         <v>68</v>
       </c>
+      <c r="C67" t="s">
+        <v>105</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
       <c r="E67">
         <v>38</v>
       </c>
@@ -1527,6 +1974,12 @@
       <c r="B68" t="s">
         <v>69</v>
       </c>
+      <c r="C68" t="s">
+        <v>95</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
       <c r="E68">
         <v>28</v>
       </c>
@@ -1538,6 +1991,12 @@
       <c r="B69" t="s">
         <v>70</v>
       </c>
+      <c r="C69" t="s">
+        <v>94</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
       <c r="E69">
         <v>36</v>
       </c>
@@ -1549,6 +2008,12 @@
       <c r="B70" t="s">
         <v>71</v>
       </c>
+      <c r="C70" t="s">
+        <v>101</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
       <c r="E70">
         <v>43</v>
       </c>
@@ -1560,6 +2025,12 @@
       <c r="B71" t="s">
         <v>72</v>
       </c>
+      <c r="C71" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
       <c r="E71">
         <v>31</v>
       </c>
@@ -1571,6 +2042,12 @@
       <c r="B72" t="s">
         <v>73</v>
       </c>
+      <c r="C72" t="s">
+        <v>104</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
       <c r="E72">
         <v>27</v>
       </c>
@@ -1582,6 +2059,12 @@
       <c r="B73" t="s">
         <v>74</v>
       </c>
+      <c r="C73" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
       <c r="E73">
         <v>32</v>
       </c>
@@ -1593,6 +2076,12 @@
       <c r="B74" t="s">
         <v>75</v>
       </c>
+      <c r="C74" t="s">
+        <v>100</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
       <c r="E74">
         <v>24</v>
       </c>
@@ -1604,6 +2093,12 @@
       <c r="B75" t="s">
         <v>76</v>
       </c>
+      <c r="C75" t="s">
+        <v>104</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
       <c r="E75">
         <v>39</v>
       </c>
@@ -1615,6 +2110,12 @@
       <c r="B76" t="s">
         <v>77</v>
       </c>
+      <c r="C76" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
       <c r="E76">
         <v>24</v>
       </c>
@@ -1625,6 +2126,12 @@
       </c>
       <c r="B77" t="s">
         <v>78</v>
+      </c>
+      <c r="C77" t="s">
+        <v>103</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
       </c>
       <c r="E77">
         <f>112+56</f>
@@ -1638,6 +2145,12 @@
       <c r="B78" t="s">
         <v>79</v>
       </c>
+      <c r="C78" t="s">
+        <v>104</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
       <c r="E78">
         <v>32</v>
       </c>
@@ -1649,6 +2162,12 @@
       <c r="B79" t="s">
         <v>80</v>
       </c>
+      <c r="C79" t="s">
+        <v>105</v>
+      </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
       <c r="E79">
         <v>40</v>
       </c>
@@ -1659,6 +2178,12 @@
       </c>
       <c r="B80" t="s">
         <v>51</v>
+      </c>
+      <c r="C80" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
       </c>
       <c r="E80">
         <f>98+30</f>
@@ -1672,6 +2197,12 @@
       <c r="B81" t="s">
         <v>11</v>
       </c>
+      <c r="C81" t="s">
+        <v>95</v>
+      </c>
+      <c r="D81">
+        <v>3</v>
+      </c>
       <c r="E81">
         <v>40</v>
       </c>
@@ -1683,6 +2214,12 @@
       <c r="B82" t="s">
         <v>81</v>
       </c>
+      <c r="C82" t="s">
+        <v>93</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
       <c r="E82">
         <v>27</v>
       </c>
@@ -1694,6 +2231,12 @@
       <c r="B83" t="s">
         <v>82</v>
       </c>
+      <c r="C83" t="s">
+        <v>103</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
       <c r="E83">
         <v>114</v>
       </c>
@@ -1705,6 +2248,12 @@
       <c r="B84" t="s">
         <v>83</v>
       </c>
+      <c r="C84" t="s">
+        <v>98</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
       <c r="E84">
         <v>16</v>
       </c>
@@ -1716,6 +2265,12 @@
       <c r="B85" t="s">
         <v>84</v>
       </c>
+      <c r="C85" t="s">
+        <v>104</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
       <c r="E85">
         <v>67</v>
       </c>
@@ -1727,6 +2282,12 @@
       <c r="B86" t="s">
         <v>85</v>
       </c>
+      <c r="C86" t="s">
+        <v>103</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
       <c r="E86">
         <v>74</v>
       </c>
@@ -1738,6 +2299,12 @@
       <c r="B87" t="s">
         <v>86</v>
       </c>
+      <c r="C87" t="s">
+        <v>105</v>
+      </c>
+      <c r="D87">
+        <v>3</v>
+      </c>
       <c r="E87">
         <v>61</v>
       </c>
@@ -1749,6 +2316,12 @@
       <c r="B88" t="s">
         <v>87</v>
       </c>
+      <c r="C88" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
       <c r="E88">
         <v>106</v>
       </c>
@@ -1760,6 +2333,12 @@
       <c r="B89" t="s">
         <v>80</v>
       </c>
+      <c r="C89" t="s">
+        <v>105</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
       <c r="E89">
         <v>81</v>
       </c>
@@ -1770,6 +2349,12 @@
       </c>
       <c r="B90" t="s">
         <v>88</v>
+      </c>
+      <c r="C90" t="s">
+        <v>106</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
       </c>
       <c r="E90">
         <v>133</v>

</xml_diff>